<commit_message>
Generated BOM, Pick-And-Place and Gerber files for JLCPCB.
</commit_message>
<xml_diff>
--- a/HARDWARE/KICAD/FABRICATION/EMBARCADOS - CURSO PCB - BOM.xlsx
+++ b/HARDWARE/KICAD/FABRICATION/EMBARCADOS - CURSO PCB - BOM.xlsx
@@ -8,19 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andre\Desktop\EMBARCADOS - CURSO PCB\HARDWARE\KICAD\FABRICATION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0485F2AF-67F6-46F5-B03E-4D2B426BAA30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA2F6CD7-BAA5-4661-93B1-E147C275AF26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{92715BCF-3C2F-4EF6-8C6E-5F9BEC51F25A}"/>
   </bookViews>
   <sheets>
     <sheet name="EMBARCADOS - CURSO PCB" sheetId="1" r:id="rId1"/>
+    <sheet name="JLCPCB - EMBARCADOS" sheetId="4" r:id="rId2"/>
+    <sheet name="JLCPCB" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="381">
   <si>
     <t>Reference</t>
   </si>
@@ -1058,6 +1073,111 @@
   </si>
   <si>
     <t xml:space="preserve">WURTH ELEKTRONIK </t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Designator</t>
+  </si>
+  <si>
+    <t>JLCPCB Part #（optional）</t>
+  </si>
+  <si>
+    <t>BatteryHolder_Keystone_1060_1x2032</t>
+  </si>
+  <si>
+    <t>C_0805_2012Metric</t>
+  </si>
+  <si>
+    <t>C_0603_1608Metric</t>
+  </si>
+  <si>
+    <t>D_SOD-123</t>
+  </si>
+  <si>
+    <t>LED_WS2812B_PLCC4_5.0x5.0mm_P3.2mm</t>
+  </si>
+  <si>
+    <t>SOT-23-6</t>
+  </si>
+  <si>
+    <t>LED_Inolux_IN-P55TATRGB_PLCC6_5.0x5.5mm_P1.8mm</t>
+  </si>
+  <si>
+    <t>L_0603_1608Metric</t>
+  </si>
+  <si>
+    <t>PinSocket_2x20_P2.54mm_Horizontal</t>
+  </si>
+  <si>
+    <t>BarrelJack_GCT_DCJ200-10-A_Horizontal</t>
+  </si>
+  <si>
+    <t>USB_C_Receptacle_G-Switch_GT-USB-7010ASV</t>
+  </si>
+  <si>
+    <t>PinSocket_2x05_P2.54mm_Horizontal</t>
+  </si>
+  <si>
+    <t>WE 693071020811</t>
+  </si>
+  <si>
+    <t>WE-LQS SMT Semi-Shielded Power Inductor</t>
+  </si>
+  <si>
+    <t>WE-CNSW SMT Common Mode Line Filter</t>
+  </si>
+  <si>
+    <t>LED_0603_1608Metric</t>
+  </si>
+  <si>
+    <t>PKM13EPYH4000-A0</t>
+  </si>
+  <si>
+    <t>SOT-23</t>
+  </si>
+  <si>
+    <t>R_0603_1608Metric</t>
+  </si>
+  <si>
+    <t>C&amp;K PTS526SM20SMTR21 LFS</t>
+  </si>
+  <si>
+    <t>TestPoint_Keystone_5000-5004_Miniature</t>
+  </si>
+  <si>
+    <t>SOT-23-5</t>
+  </si>
+  <si>
+    <t>SOT-223-3_TabPin2</t>
+  </si>
+  <si>
+    <t>TSSOP-14_4.4x5mm_P0.65mm</t>
+  </si>
+  <si>
+    <t>TSSOP-10_3x3mm_P0.5mm</t>
+  </si>
+  <si>
+    <t>OLED 128x64 1.3in</t>
+  </si>
+  <si>
+    <t>LQFP-64_10x10mm_P0.5mm</t>
+  </si>
+  <si>
+    <t>Crystal_SMD_3215-2Pin_3.2x1.5mm</t>
+  </si>
+  <si>
+    <t>Crystal_SMD_3225-4Pin_3.2x2.5mm</t>
+  </si>
+  <si>
+    <t>C318884</t>
+  </si>
+  <si>
+    <t>TS-1187A-B-A-B</t>
+  </si>
+  <si>
+    <t>XKB Connection</t>
   </si>
 </sst>
 </file>
@@ -1381,7 +1501,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -1496,6 +1616,117 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1541,9 +1772,21 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1589,7 +1832,133 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -1615,18 +1984,77 @@
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{5DEB532D-54A4-486C-910F-12CC83A32484}" name="#"/>
     <tableColumn id="2" xr3:uid="{6172368D-786D-48E1-80C4-A9CD7E00E4CE}" name="Reference"/>
-    <tableColumn id="3" xr3:uid="{F9438533-A33B-4C22-82D3-70AE3C601589}" name="Value" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{F9438533-A33B-4C22-82D3-70AE3C601589}" name="Value" dataDxfId="9"/>
     <tableColumn id="4" xr3:uid="{9C0A32FF-D9ED-445E-803E-B200327292B7}" name="Datasheet"/>
     <tableColumn id="5" xr3:uid="{0E03777B-A907-4D2F-9089-F54ACCA4305E}" name="Footprint"/>
     <tableColumn id="6" xr3:uid="{E270BBB9-FD82-4E77-B068-AA4A945224BC}" name="Qty"/>
     <tableColumn id="7" xr3:uid="{99C1B04C-E267-43F1-AFB7-6AF5C3391DE2}" name="3D Model"/>
-    <tableColumn id="8" xr3:uid="{95CC667A-E12A-4BD2-B863-5A8F7D62B8FE}" name="MPN" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{95CC667A-E12A-4BD2-B863-5A8F7D62B8FE}" name="MPN" dataDxfId="8"/>
     <tableColumn id="9" xr3:uid="{2B23A03C-969F-4CB6-8B09-75479ED76A45}" name="Manufacturer"/>
     <tableColumn id="10" xr3:uid="{A80CBF62-DA6E-4F9D-9F67-7593F46D4E0F}" name="Notes"/>
     <tableColumn id="11" xr3:uid="{2FCA9081-C6EA-49FE-827D-ADF2A8DA0610}" name="LCSC MANUFACTURER "/>
     <tableColumn id="12" xr3:uid="{E44437BA-FAC9-456F-A422-41D0E696FBE1}" name="LCSC MPN "/>
     <tableColumn id="13" xr3:uid="{81D3DE6A-5AC6-49DF-A90B-04FFC79AB08F}" name="LCSC Part # "/>
     <tableColumn id="14" xr3:uid="{127BC9BE-0489-4062-AEAB-0E4D6E62EAB7}" name="Description"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{39B4C106-F6F0-4AB0-A05F-DA51ED0F2CA8}" name="Table3" displayName="Table3" ref="A1:D59" totalsRowShown="0">
+  <autoFilter ref="A1:D59" xr:uid="{39B4C106-F6F0-4AB0-A05F-DA51ED0F2CA8}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="C128052"/>
+        <filter val="C14663"/>
+        <filter val="C15850"/>
+        <filter val="C1634"/>
+        <filter val="C19189038"/>
+        <filter val="C21189"/>
+        <filter val="C21190"/>
+        <filter val="C23186"/>
+        <filter val="C23197"/>
+        <filter val="C25804"/>
+        <filter val="C2827654"/>
+        <filter val="C2827672"/>
+        <filter val="C2927038"/>
+        <filter val="C318884"/>
+        <filter val="C327005"/>
+        <filter val="C37593"/>
+        <filter val="C398929"/>
+        <filter val="C4190"/>
+        <filter val="C460356"/>
+        <filter val="C520138"/>
+        <filter val="C5563819"/>
+        <filter val="C6071564"/>
+        <filter val="C6186"/>
+        <filter val="C6187"/>
+        <filter val="C82544"/>
+        <filter val="C8545"/>
+        <filter val="C94355"/>
+        <filter val="C963865"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{784E5981-BB71-489A-9D63-0779120936CF}" name="Comment"/>
+    <tableColumn id="2" xr3:uid="{86671218-2B4F-4E8B-8435-113024F082AB}" name="Designator"/>
+    <tableColumn id="3" xr3:uid="{1FD16CE3-7127-447D-8CCD-5E6BF1EC2F05}" name="Footprint"/>
+    <tableColumn id="4" xr3:uid="{29C424C1-012D-4A06-A631-FA03FD132CFF}" name="JLCPCB Part #（optional）"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A563B893-C1FA-4972-9E76-7201D0F49F1E}" name="Table2" displayName="Table2" ref="A1:D59" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="6" tableBorderDxfId="7" totalsRowBorderDxfId="5">
+  <autoFilter ref="A1:D59" xr:uid="{A563B893-C1FA-4972-9E76-7201D0F49F1E}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{2341E0EF-897B-4EB5-BACD-6385C331045B}" name="Comment" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{B0059D76-D071-4FCC-9930-28633FBCA0C6}" name="Designator" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{59C7656D-4ACA-4B2E-9663-CA24E303CC98}" name="Footprint" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{B239057C-C119-44E5-B366-7F91E1DFFA1F}" name="JLCPCB Part #（optional）" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1951,20 +2379,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFB4FC3A-D128-45CD-BB50-23A5834C3414}">
   <dimension ref="A1:N59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.140625" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" style="1"/>
+    <col min="5" max="5" width="30" customWidth="1"/>
     <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" style="1" customWidth="1"/>
     <col min="9" max="9" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="31.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="23" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.140625" customWidth="1"/>
-    <col min="14" max="14" width="163" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="42.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -3266,13 +3698,13 @@
         <v>19</v>
       </c>
       <c r="K30" t="s">
-        <v>19</v>
-      </c>
-      <c r="L30" t="s">
-        <v>19</v>
+        <v>380</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>379</v>
       </c>
       <c r="M30" t="s">
-        <v>19</v>
+        <v>378</v>
       </c>
       <c r="N30" t="s">
         <v>223</v>
@@ -3310,13 +3742,13 @@
         <v>19</v>
       </c>
       <c r="K31" t="s">
-        <v>19</v>
-      </c>
-      <c r="L31" t="s">
-        <v>19</v>
+        <v>380</v>
+      </c>
+      <c r="L31" s="3" t="s">
+        <v>379</v>
       </c>
       <c r="M31" t="s">
-        <v>19</v>
+        <v>378</v>
       </c>
       <c r="N31" t="s">
         <v>223</v>
@@ -3354,13 +3786,13 @@
         <v>19</v>
       </c>
       <c r="K32" t="s">
-        <v>19</v>
-      </c>
-      <c r="L32" t="s">
-        <v>19</v>
+        <v>380</v>
+      </c>
+      <c r="L32" s="3" t="s">
+        <v>379</v>
       </c>
       <c r="M32" t="s">
-        <v>19</v>
+        <v>378</v>
       </c>
       <c r="N32" t="s">
         <v>223</v>
@@ -3398,13 +3830,13 @@
         <v>19</v>
       </c>
       <c r="K33" t="s">
-        <v>19</v>
-      </c>
-      <c r="L33" t="s">
-        <v>19</v>
+        <v>380</v>
+      </c>
+      <c r="L33" s="3" t="s">
+        <v>379</v>
       </c>
       <c r="M33" t="s">
-        <v>19</v>
+        <v>378</v>
       </c>
       <c r="N33" t="s">
         <v>223</v>
@@ -3442,13 +3874,13 @@
         <v>19</v>
       </c>
       <c r="K34" t="s">
-        <v>19</v>
-      </c>
-      <c r="L34" t="s">
-        <v>19</v>
+        <v>380</v>
+      </c>
+      <c r="L34" s="3" t="s">
+        <v>379</v>
       </c>
       <c r="M34" t="s">
-        <v>19</v>
+        <v>378</v>
       </c>
       <c r="N34" t="s">
         <v>223</v>
@@ -3486,13 +3918,13 @@
         <v>19</v>
       </c>
       <c r="K35" t="s">
-        <v>19</v>
-      </c>
-      <c r="L35" t="s">
-        <v>19</v>
+        <v>380</v>
+      </c>
+      <c r="L35" s="3" t="s">
+        <v>379</v>
       </c>
       <c r="M35" t="s">
-        <v>19</v>
+        <v>378</v>
       </c>
       <c r="N35" t="s">
         <v>223</v>
@@ -3530,13 +3962,13 @@
         <v>19</v>
       </c>
       <c r="K36" t="s">
-        <v>19</v>
-      </c>
-      <c r="L36" t="s">
-        <v>19</v>
+        <v>380</v>
+      </c>
+      <c r="L36" s="3" t="s">
+        <v>379</v>
       </c>
       <c r="M36" t="s">
-        <v>19</v>
+        <v>378</v>
       </c>
       <c r="N36" t="s">
         <v>223</v>
@@ -3574,13 +4006,13 @@
         <v>19</v>
       </c>
       <c r="K37" t="s">
-        <v>19</v>
-      </c>
-      <c r="L37" t="s">
-        <v>19</v>
+        <v>380</v>
+      </c>
+      <c r="L37" s="3" t="s">
+        <v>379</v>
       </c>
       <c r="M37" t="s">
-        <v>19</v>
+        <v>378</v>
       </c>
       <c r="N37" t="s">
         <v>223</v>
@@ -3618,13 +4050,13 @@
         <v>19</v>
       </c>
       <c r="K38" t="s">
-        <v>19</v>
-      </c>
-      <c r="L38" t="s">
-        <v>19</v>
+        <v>380</v>
+      </c>
+      <c r="L38" s="3" t="s">
+        <v>379</v>
       </c>
       <c r="M38" t="s">
-        <v>19</v>
+        <v>378</v>
       </c>
       <c r="N38" t="s">
         <v>223</v>
@@ -4300,6 +4732,1670 @@
       </c>
       <c r="N59" t="s">
         <v>330</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79D1ACFC-4CBF-4815-869D-84F3D447EBAA}">
+  <dimension ref="A1:D59"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D59" sqref="A1:D59"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="40.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="74.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>346</v>
+      </c>
+      <c r="B1" t="s">
+        <v>347</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>349</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>350</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>351</v>
+      </c>
+      <c r="D4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>351</v>
+      </c>
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" t="s">
+        <v>351</v>
+      </c>
+      <c r="D6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" t="s">
+        <v>352</v>
+      </c>
+      <c r="D7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" t="s">
+        <v>353</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" t="s">
+        <v>354</v>
+      </c>
+      <c r="D9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" t="s">
+        <v>354</v>
+      </c>
+      <c r="D10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" t="s">
+        <v>355</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>95</v>
+      </c>
+      <c r="B12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" t="s">
+        <v>356</v>
+      </c>
+      <c r="D12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C13" t="s">
+        <v>357</v>
+      </c>
+      <c r="D13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>108</v>
+      </c>
+      <c r="B14" t="s">
+        <v>103</v>
+      </c>
+      <c r="C14" t="s">
+        <v>358</v>
+      </c>
+      <c r="D14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>117</v>
+      </c>
+      <c r="B15" t="s">
+        <v>109</v>
+      </c>
+      <c r="C15" t="s">
+        <v>359</v>
+      </c>
+      <c r="D15" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>123</v>
+      </c>
+      <c r="B16" t="s">
+        <v>118</v>
+      </c>
+      <c r="C16" t="s">
+        <v>360</v>
+      </c>
+      <c r="D16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>132</v>
+      </c>
+      <c r="B17" t="s">
+        <v>124</v>
+      </c>
+      <c r="C17" t="s">
+        <v>361</v>
+      </c>
+      <c r="D17" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>140</v>
+      </c>
+      <c r="B18" t="s">
+        <v>133</v>
+      </c>
+      <c r="C18" t="s">
+        <v>362</v>
+      </c>
+      <c r="D18" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>146</v>
+      </c>
+      <c r="B19" t="s">
+        <v>141</v>
+      </c>
+      <c r="C19" t="s">
+        <v>363</v>
+      </c>
+      <c r="D19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>155</v>
+      </c>
+      <c r="B20" t="s">
+        <v>147</v>
+      </c>
+      <c r="C20" t="s">
+        <v>364</v>
+      </c>
+      <c r="D20" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>162</v>
+      </c>
+      <c r="B21" t="s">
+        <v>156</v>
+      </c>
+      <c r="C21" t="s">
+        <v>365</v>
+      </c>
+      <c r="D21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>171</v>
+      </c>
+      <c r="B22" t="s">
+        <v>163</v>
+      </c>
+      <c r="C22" t="s">
+        <v>366</v>
+      </c>
+      <c r="D22" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>181</v>
+      </c>
+      <c r="B23" t="s">
+        <v>172</v>
+      </c>
+      <c r="C23" t="s">
+        <v>367</v>
+      </c>
+      <c r="D23" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>185</v>
+      </c>
+      <c r="B24" t="s">
+        <v>182</v>
+      </c>
+      <c r="C24" t="s">
+        <v>367</v>
+      </c>
+      <c r="D24" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>191</v>
+      </c>
+      <c r="B25" t="s">
+        <v>186</v>
+      </c>
+      <c r="C25" t="s">
+        <v>367</v>
+      </c>
+      <c r="D25" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>197</v>
+      </c>
+      <c r="B26" t="s">
+        <v>192</v>
+      </c>
+      <c r="C26" t="s">
+        <v>367</v>
+      </c>
+      <c r="D26" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>203</v>
+      </c>
+      <c r="B27" t="s">
+        <v>198</v>
+      </c>
+      <c r="C27" t="s">
+        <v>367</v>
+      </c>
+      <c r="D27" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>209</v>
+      </c>
+      <c r="B28" t="s">
+        <v>204</v>
+      </c>
+      <c r="C28" t="s">
+        <v>367</v>
+      </c>
+      <c r="D28" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>215</v>
+      </c>
+      <c r="B29" t="s">
+        <v>210</v>
+      </c>
+      <c r="C29" t="s">
+        <v>367</v>
+      </c>
+      <c r="D29" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>223</v>
+      </c>
+      <c r="B30" t="s">
+        <v>216</v>
+      </c>
+      <c r="C30" t="s">
+        <v>368</v>
+      </c>
+      <c r="D30" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>223</v>
+      </c>
+      <c r="B31" t="s">
+        <v>224</v>
+      </c>
+      <c r="C31" t="s">
+        <v>368</v>
+      </c>
+      <c r="D31" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>223</v>
+      </c>
+      <c r="B32" t="s">
+        <v>226</v>
+      </c>
+      <c r="C32" t="s">
+        <v>368</v>
+      </c>
+      <c r="D32" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>223</v>
+      </c>
+      <c r="B33" t="s">
+        <v>228</v>
+      </c>
+      <c r="C33" t="s">
+        <v>368</v>
+      </c>
+      <c r="D33" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>223</v>
+      </c>
+      <c r="B34" t="s">
+        <v>230</v>
+      </c>
+      <c r="C34" t="s">
+        <v>368</v>
+      </c>
+      <c r="D34" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>223</v>
+      </c>
+      <c r="B35" t="s">
+        <v>232</v>
+      </c>
+      <c r="C35" t="s">
+        <v>368</v>
+      </c>
+      <c r="D35" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>223</v>
+      </c>
+      <c r="B36" t="s">
+        <v>234</v>
+      </c>
+      <c r="C36" t="s">
+        <v>368</v>
+      </c>
+      <c r="D36" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>223</v>
+      </c>
+      <c r="B37" t="s">
+        <v>236</v>
+      </c>
+      <c r="C37" t="s">
+        <v>368</v>
+      </c>
+      <c r="D37" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>223</v>
+      </c>
+      <c r="B38" t="s">
+        <v>238</v>
+      </c>
+      <c r="C38" t="s">
+        <v>368</v>
+      </c>
+      <c r="D38" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>243</v>
+      </c>
+      <c r="B39" t="s">
+        <v>240</v>
+      </c>
+      <c r="C39" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>243</v>
+      </c>
+      <c r="B40" t="s">
+        <v>244</v>
+      </c>
+      <c r="C40" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>243</v>
+      </c>
+      <c r="B41" t="s">
+        <v>246</v>
+      </c>
+      <c r="C41" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>243</v>
+      </c>
+      <c r="B42" t="s">
+        <v>248</v>
+      </c>
+      <c r="C42" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>243</v>
+      </c>
+      <c r="B43" t="s">
+        <v>249</v>
+      </c>
+      <c r="C43" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>243</v>
+      </c>
+      <c r="B44" t="s">
+        <v>250</v>
+      </c>
+      <c r="C44" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>243</v>
+      </c>
+      <c r="B45" t="s">
+        <v>252</v>
+      </c>
+      <c r="C45" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>243</v>
+      </c>
+      <c r="B46" t="s">
+        <v>254</v>
+      </c>
+      <c r="C46" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>243</v>
+      </c>
+      <c r="B47" t="s">
+        <v>255</v>
+      </c>
+      <c r="C47" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>243</v>
+      </c>
+      <c r="B48" t="s">
+        <v>257</v>
+      </c>
+      <c r="C48" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>243</v>
+      </c>
+      <c r="B49" t="s">
+        <v>258</v>
+      </c>
+      <c r="C49" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>243</v>
+      </c>
+      <c r="B50" t="s">
+        <v>260</v>
+      </c>
+      <c r="C50" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>268</v>
+      </c>
+      <c r="B51" t="s">
+        <v>261</v>
+      </c>
+      <c r="C51" t="s">
+        <v>370</v>
+      </c>
+      <c r="D51" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>277</v>
+      </c>
+      <c r="B52" t="s">
+        <v>269</v>
+      </c>
+      <c r="C52" t="s">
+        <v>371</v>
+      </c>
+      <c r="D52" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>283</v>
+      </c>
+      <c r="B53" t="s">
+        <v>278</v>
+      </c>
+      <c r="C53" t="s">
+        <v>371</v>
+      </c>
+      <c r="D53" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>292</v>
+      </c>
+      <c r="B54" t="s">
+        <v>284</v>
+      </c>
+      <c r="C54" t="s">
+        <v>372</v>
+      </c>
+      <c r="D54" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>299</v>
+      </c>
+      <c r="B55" t="s">
+        <v>293</v>
+      </c>
+      <c r="C55" t="s">
+        <v>373</v>
+      </c>
+      <c r="D55" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>301</v>
+      </c>
+      <c r="B56" t="s">
+        <v>300</v>
+      </c>
+      <c r="C56" t="s">
+        <v>374</v>
+      </c>
+      <c r="D56" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>311</v>
+      </c>
+      <c r="B57" t="s">
+        <v>304</v>
+      </c>
+      <c r="C57" t="s">
+        <v>375</v>
+      </c>
+      <c r="D57" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>321</v>
+      </c>
+      <c r="B58" t="s">
+        <v>312</v>
+      </c>
+      <c r="C58" t="s">
+        <v>376</v>
+      </c>
+      <c r="D58" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>330</v>
+      </c>
+      <c r="B59" t="s">
+        <v>322</v>
+      </c>
+      <c r="C59" t="s">
+        <v>377</v>
+      </c>
+      <c r="D59" t="s">
+        <v>328</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1087F916-4AC9-446E-BA1B-D66ED3F37ABD}">
+  <dimension ref="A1:D59"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A56" sqref="A56:D56"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="115.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="9" t="s">
+        <v>330</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>322</v>
+      </c>
+      <c r="C59" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="D59" s="11" t="s">
+        <v>328</v>
       </c>
     </row>
   </sheetData>

</xml_diff>